<commit_message>
updating excel and csvs
</commit_message>
<xml_diff>
--- a/data/datacollectionmonths.xlsx
+++ b/data/datacollectionmonths.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/Dropbox/GRADSCHOOL/Dissertation/R_dissertation/Ch3_piru_enhancement_Git/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephaniema/Dropbox/GRADSCHOOL/Dissertation/R_dissertation/Ch3_piru_enhancement_Git/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F328067E-ECE6-DE40-AF89-FDD430D46988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A04C2AE-CA3C-EE4A-A9C9-CB3BC06D8F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35780" yWindow="960" windowWidth="27640" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datacollectionmonths" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="18">
   <si>
     <t>year_1</t>
   </si>
@@ -70,11 +70,17 @@
   <si>
     <t>survey</t>
   </si>
+  <si>
+    <t>WINTER PAR, WINTER TDR --&gt; predict spring survival, predict summer survival</t>
+  </si>
+  <si>
+    <t>SPRING PAR, SPRING TDR --&gt; predict summer survival</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -558,10 +564,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -916,7 +921,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1761,19 +1766,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="5" max="10" width="10.83203125" style="2"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1786,23 +1788,23 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>2018</v>
       </c>
@@ -1812,14 +1814,14 @@
       <c r="D2">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>2018</v>
       </c>
@@ -1829,14 +1831,14 @@
       <c r="D3">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2018</v>
       </c>
@@ -1847,7 +1849,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1860,14 +1862,17 @@
       <c r="D5">
         <v>15</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1880,17 +1885,17 @@
       <c r="D6">
         <v>16</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="2" t="s">
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>2018</v>
       </c>
@@ -1901,7 +1906,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>2018</v>
       </c>
@@ -1912,7 +1917,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>2018</v>
       </c>
@@ -1923,7 +1928,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>2018</v>
       </c>
@@ -1933,11 +1938,11 @@
       <c r="D10">
         <v>20</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>2018</v>
       </c>
@@ -1948,7 +1953,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>2018</v>
       </c>
@@ -1959,7 +1964,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>2018</v>
       </c>
@@ -1969,17 +1974,20 @@
       <c r="D13">
         <v>23</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="2" t="s">
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>2019</v>
       </c>
@@ -1989,17 +1997,17 @@
       <c r="D14">
         <v>24</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>2019</v>
       </c>
@@ -2009,8 +2017,11 @@
       <c r="D15">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>2019</v>
       </c>
@@ -2020,20 +2031,20 @@
       <c r="D16">
         <v>26</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>2019</v>
       </c>
@@ -2054,16 +2065,16 @@
       <c r="D18">
         <v>28</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="2" t="s">
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" t="s">
         <v>8</v>
       </c>
       <c r="K18" t="s">
@@ -2080,10 +2091,10 @@
       <c r="D19">
         <v>29</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="2" t="s">
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2097,7 +2108,7 @@
       <c r="D20">
         <v>30</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2122,13 +2133,13 @@
       <c r="D22">
         <v>32</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="2" t="s">
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2153,13 +2164,13 @@
       <c r="D24">
         <v>34</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="2" t="s">
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2206,13 +2217,13 @@
       <c r="D28">
         <v>38</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="2" t="s">
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2226,7 +2237,7 @@
       <c r="D29">
         <v>39</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H29" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2240,13 +2251,13 @@
       <c r="D30">
         <v>40</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" s="2" t="s">
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2304,10 +2315,10 @@
       <c r="D35">
         <v>45</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="2" t="s">
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2354,10 +2365,10 @@
       <c r="D39">
         <v>49</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="2" t="s">
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2382,10 +2393,10 @@
       <c r="D41">
         <v>51</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="2" t="s">
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>